<commit_message>
create function for tg bot
</commit_message>
<xml_diff>
--- a/dataframes.xlsx
+++ b/dataframes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snegu\Documents\Hacks\Vacancy-Handler-Roskapstroy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002F9BE0-24CE-46D3-82BA-51F4AF23C490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E623B4E-865A-4274-98B6-1B7DF46E9F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -466,78 +466,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.5546875" customWidth="1"/>
-    <col min="3" max="3" width="40.44140625" customWidth="1"/>
-    <col min="4" max="4" width="35.77734375" customWidth="1"/>
-    <col min="5" max="5" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="288" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>0</v>
+    <row r="3" spans="1:4" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>0</v>
+    <row r="4" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>